<commit_message>
Preise + Excel Vorlage geändert + README ergänzt
</commit_message>
<xml_diff>
--- a/HS23_DC-Script_PSIA416_Excel-Vorlage_230114.xlsx
+++ b/HS23_DC-Script_PSIA416_Excel-Vorlage_230114.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m.amstad/Documents/Python Grundlagen/Project-SIA-416/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405BBA8C-0961-5945-A406-DF605A2D8DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E13F08-31D7-B240-8AA5-A7D4A1C6A8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{CBFEDF2E-64E9-446E-94A7-D21275BF08BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -118,9 +118,6 @@
     <t>+/- 20% genau</t>
   </si>
   <si>
-    <t>Auszug der Flächen und Volumen des Projektmodelles nach SIA 416</t>
-  </si>
-  <si>
     <t>Nutzfläche
 NF</t>
   </si>
@@ -178,15 +175,18 @@
 NV</t>
   </si>
   <si>
-    <t>Grobkostenschätzung</t>
-  </si>
-  <si>
     <t>nach</t>
   </si>
   <si>
     <t>Aussen-
 Funktionsfläche 
 AF</t>
+  </si>
+  <si>
+    <t>Grobkostenschätzung BKP 2</t>
+  </si>
+  <si>
+    <t>Auszug der Flächen und Volumen des Projektmodells nach SIA 416</t>
   </si>
 </sst>
 </file>
@@ -194,7 +194,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="#,##0\ &quot;CHF&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;CHF&quot;"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -502,29 +502,149 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -546,135 +666,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3305D52F-5990-48CF-B074-B90189145B53}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2095,13 +2095,13 @@
       <c r="A1" s="1" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
       <c r="E1" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>0</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -2125,9 +2125,9 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="83" t="str">
+      <c r="F3" s="28" t="str">
         <f ca="1">TEXT(TODAY(), "TT.MM.JJJJ")</f>
-        <v>14.01.2024</v>
+        <v>15.01.2024</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16">
@@ -2152,7 +2152,7 @@
     </row>
     <row r="6" spans="1:6" ht="16">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2169,102 +2169,102 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.25" customHeight="1">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="73"/>
     </row>
     <row r="9" spans="1:6" ht="15.25" customHeight="1">
-      <c r="A9" s="68">
+      <c r="A9" s="36">
         <v>0</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" ht="16">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="35" t="s">
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="78"/>
     </row>
     <row r="11" spans="1:6" ht="16">
-      <c r="A11" s="49">
+      <c r="A11" s="79">
         <v>0</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52">
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="45">
         <f>(A9-A11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="53"/>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" spans="1:6" ht="48">
-      <c r="A12" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56" t="s">
+      <c r="A12" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="83"/>
+      <c r="C12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="59"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="60">
+      <c r="A13" s="51">
         <f>SUM(A15,B15)</f>
         <v>0</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="60">
+      <c r="B13" s="52"/>
+      <c r="C13" s="51">
         <v>0</v>
       </c>
-      <c r="D13" s="60">
+      <c r="D13" s="51">
         <v>0</v>
       </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="59"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:6" ht="43.75" customHeight="1">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:6" ht="15.25" customHeight="1">
-      <c r="A15" s="64">
+      <c r="A15" s="24">
         <v>0</v>
       </c>
-      <c r="B15" s="64">
+      <c r="B15" s="24">
         <v>0</v>
       </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="67"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:6" ht="22.5" customHeight="1">
       <c r="A16" s="3"/>
@@ -2275,60 +2275,60 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.25" customHeight="1">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="73"/>
     </row>
     <row r="18" spans="1:6" ht="15.25" customHeight="1">
-      <c r="A18" s="43">
+      <c r="A18" s="39">
         <v>0</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="45"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="1:6" ht="16">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35" t="s">
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="36"/>
+      <c r="F19" s="78"/>
     </row>
     <row r="20" spans="1:6" ht="16">
-      <c r="A20" s="49">
+      <c r="A20" s="79">
         <f>SUM(A22,C22,D22)</f>
         <v>0</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="68">
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="36">
         <v>0</v>
       </c>
-      <c r="F20" s="70"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="48">
-      <c r="A21" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="26"/>
+      <c r="A21" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="58"/>
       <c r="C21" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>10</v>
@@ -2338,20 +2338,20 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="71">
+      <c r="A22" s="69">
         <v>0</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="64">
+      <c r="B22" s="70"/>
+      <c r="C22" s="24">
         <v>0</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D22" s="24">
         <v>0</v>
       </c>
-      <c r="E22" s="64">
+      <c r="E22" s="24">
         <v>0</v>
       </c>
-      <c r="F22" s="73">
+      <c r="F22" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2363,76 +2363,76 @@
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="16">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" spans="1:6" ht="16">
-      <c r="A25" s="23">
+      <c r="A25" s="42">
         <v>0</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="46"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44"/>
     </row>
     <row r="26" spans="1:6" ht="16">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="40" t="s">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="41"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:6" ht="16">
-      <c r="A27" s="23">
+      <c r="A27" s="42">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="77">
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="59">
         <v>0</v>
       </c>
-      <c r="F27" s="78"/>
+      <c r="F27" s="60"/>
     </row>
     <row r="28" spans="1:6" ht="48">
       <c r="A28" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="80"/>
+      <c r="C28" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="66"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="62"/>
     </row>
     <row r="29" spans="1:6" ht="15.5" customHeight="1">
-      <c r="A29" s="74">
+      <c r="A29" s="27">
         <v>0</v>
       </c>
-      <c r="B29" s="74">
+      <c r="B29" s="27">
         <v>0</v>
       </c>
-      <c r="C29" s="75">
+      <c r="C29" s="67">
         <v>0</v>
       </c>
-      <c r="D29" s="76"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="82"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="64"/>
     </row>
     <row r="30" spans="1:6" ht="22.75" customHeight="1">
       <c r="A30" s="11"/>
@@ -2441,12 +2441,12 @@
     </row>
     <row r="31" spans="1:6" ht="16">
       <c r="A31" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
-      <c r="D31" s="47" t="s">
-        <v>33</v>
+      <c r="D31" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>13</v>
@@ -2461,14 +2461,14 @@
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="48">
+      <c r="A33" s="29">
         <v>0</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:6" ht="22.75" customHeight="1"/>
     <row r="35" spans="1:6">
@@ -2478,18 +2478,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="E11:F15"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A21:B21"/>
@@ -2506,6 +2494,18 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="E11:F15"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
   </mergeCells>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>